<commit_message>
export Data to SQL Tagle
</commit_message>
<xml_diff>
--- a/Results/OLS_Results_Top.xlsx
+++ b/Results/OLS_Results_Top.xlsx
@@ -1402,7 +1402,7 @@
     <t>HAC</t>
   </si>
   <si>
-    <t>Wed, 13 Apr 2022</t>
+    <t>Tue, 03 May 2022</t>
   </si>
   <si>
     <t>CLc1</t>
@@ -5110,19 +5110,19 @@
     <t>0.284</t>
   </si>
   <si>
-    <t>06:45:58</t>
-  </si>
-  <si>
-    <t>06:45:59</t>
-  </si>
-  <si>
-    <t>06:46:00</t>
-  </si>
-  <si>
-    <t>06:46:01</t>
-  </si>
-  <si>
-    <t>06:46:02</t>
+    <t>08:07:54</t>
+  </si>
+  <si>
+    <t>08:07:53</t>
+  </si>
+  <si>
+    <t>08:07:55</t>
+  </si>
+  <si>
+    <t>08:07:56</t>
+  </si>
+  <si>
+    <t>08:07:57</t>
   </si>
 </sst>
 </file>
@@ -5715,7 +5715,7 @@
         <v>1587</v>
       </c>
       <c r="Z3" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -5792,7 +5792,7 @@
         <v>1290</v>
       </c>
       <c r="Z4" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -5869,7 +5869,7 @@
         <v>1588</v>
       </c>
       <c r="Z5" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -5946,7 +5946,7 @@
         <v>1589</v>
       </c>
       <c r="Z6" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -6023,7 +6023,7 @@
         <v>1590</v>
       </c>
       <c r="Z7" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -6100,7 +6100,7 @@
         <v>1591</v>
       </c>
       <c r="Z8" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="9" spans="1:26">
@@ -6177,7 +6177,7 @@
         <v>1592</v>
       </c>
       <c r="Z9" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -6254,7 +6254,7 @@
         <v>1593</v>
       </c>
       <c r="Z10" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -6331,7 +6331,7 @@
         <v>1594</v>
       </c>
       <c r="Z11" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="12" spans="1:26">
@@ -6639,7 +6639,7 @@
         <v>1598</v>
       </c>
       <c r="Z15" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="16" spans="1:26">
@@ -7024,7 +7024,7 @@
         <v>1603</v>
       </c>
       <c r="Z20" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="21" spans="1:26">
@@ -7101,7 +7101,7 @@
         <v>1604</v>
       </c>
       <c r="Z21" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="22" spans="1:26">
@@ -7178,7 +7178,7 @@
         <v>1605</v>
       </c>
       <c r="Z22" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="23" spans="1:26">
@@ -7255,7 +7255,7 @@
         <v>1606</v>
       </c>
       <c r="Z23" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="24" spans="1:26">
@@ -7332,7 +7332,7 @@
         <v>1607</v>
       </c>
       <c r="Z24" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="25" spans="1:26">
@@ -7409,7 +7409,7 @@
         <v>1608</v>
       </c>
       <c r="Z25" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="26" spans="1:26">
@@ -7486,7 +7486,7 @@
         <v>1609</v>
       </c>
       <c r="Z26" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="27" spans="1:26">
@@ -7563,7 +7563,7 @@
         <v>1610</v>
       </c>
       <c r="Z27" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="28" spans="1:26">
@@ -7640,7 +7640,7 @@
         <v>1584</v>
       </c>
       <c r="Z28" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="29" spans="1:26">
@@ -7717,7 +7717,7 @@
         <v>319</v>
       </c>
       <c r="Z29" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="30" spans="1:26">
@@ -7794,7 +7794,7 @@
         <v>1576</v>
       </c>
       <c r="Z30" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="31" spans="1:26">
@@ -7871,7 +7871,7 @@
         <v>304</v>
       </c>
       <c r="Z31" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="32" spans="1:26">
@@ -7948,7 +7948,7 @@
         <v>1611</v>
       </c>
       <c r="Z32" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="33" spans="1:26">
@@ -8025,7 +8025,7 @@
         <v>337</v>
       </c>
       <c r="Z33" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="34" spans="1:26">
@@ -8102,7 +8102,7 @@
         <v>329</v>
       </c>
       <c r="Z34" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="35" spans="1:26">
@@ -8179,7 +8179,7 @@
         <v>1612</v>
       </c>
       <c r="Z35" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="36" spans="1:26">
@@ -8256,7 +8256,7 @@
         <v>294</v>
       </c>
       <c r="Z36" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="37" spans="1:26">
@@ -8333,7 +8333,7 @@
         <v>1613</v>
       </c>
       <c r="Z37" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="38" spans="1:26">
@@ -8410,7 +8410,7 @@
         <v>307</v>
       </c>
       <c r="Z38" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="39" spans="1:26">
@@ -8487,7 +8487,7 @@
         <v>326</v>
       </c>
       <c r="Z39" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="40" spans="1:26">
@@ -8564,7 +8564,7 @@
         <v>328</v>
       </c>
       <c r="Z40" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="41" spans="1:26">
@@ -8718,7 +8718,7 @@
         <v>1615</v>
       </c>
       <c r="Z42" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="43" spans="1:26">
@@ -8795,7 +8795,7 @@
         <v>1616</v>
       </c>
       <c r="Z43" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="44" spans="1:26">
@@ -8872,7 +8872,7 @@
         <v>1617</v>
       </c>
       <c r="Z44" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="45" spans="1:26">
@@ -8949,7 +8949,7 @@
         <v>1618</v>
       </c>
       <c r="Z45" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="46" spans="1:26">
@@ -9026,7 +9026,7 @@
         <v>1619</v>
       </c>
       <c r="Z46" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="47" spans="1:26">
@@ -9103,7 +9103,7 @@
         <v>1620</v>
       </c>
       <c r="Z47" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="48" spans="1:26">
@@ -9180,7 +9180,7 @@
         <v>1621</v>
       </c>
       <c r="Z48" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="49" spans="1:26">
@@ -9257,7 +9257,7 @@
         <v>1622</v>
       </c>
       <c r="Z49" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="50" spans="1:26">
@@ -9334,7 +9334,7 @@
         <v>1623</v>
       </c>
       <c r="Z50" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="51" spans="1:26">
@@ -9411,7 +9411,7 @@
         <v>1624</v>
       </c>
       <c r="Z51" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="52" spans="1:26">
@@ -9488,7 +9488,7 @@
         <v>1618</v>
       </c>
       <c r="Z52" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="53" spans="1:26">
@@ -9565,7 +9565,7 @@
         <v>1625</v>
       </c>
       <c r="Z53" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
     </row>
     <row r="54" spans="1:26">
@@ -13646,7 +13646,7 @@
         <v>325</v>
       </c>
       <c r="Z106" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="107" spans="1:26">
@@ -14185,7 +14185,7 @@
         <v>1671</v>
       </c>
       <c r="Z113" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="114" spans="1:26">
@@ -14262,7 +14262,7 @@
         <v>1672</v>
       </c>
       <c r="Z114" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="115" spans="1:26">
@@ -14339,7 +14339,7 @@
         <v>1602</v>
       </c>
       <c r="Z115" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="116" spans="1:26">
@@ -14416,7 +14416,7 @@
         <v>1673</v>
       </c>
       <c r="Z116" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="117" spans="1:26">
@@ -14493,7 +14493,7 @@
         <v>1674</v>
       </c>
       <c r="Z117" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="118" spans="1:26">
@@ -14570,7 +14570,7 @@
         <v>1675</v>
       </c>
       <c r="Z118" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="119" spans="1:26">
@@ -14724,7 +14724,7 @@
         <v>1677</v>
       </c>
       <c r="Z120" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="121" spans="1:26">

</xml_diff>